<commit_message>
the design of product reports has been improved
</commit_message>
<xml_diff>
--- a/excel/reporte_producto.xlsx
+++ b/excel/reporte_producto.xlsx
@@ -7,7 +7,7 @@
     <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Worksheet" sheetId="1" r:id="rId4"/>
+    <sheet name="Reporte Productos" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
@@ -15,30 +15,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
+  <si>
+    <t>Reporte de Ventas</t>
+  </si>
+  <si>
+    <t>Fecha  2021-11-18 15:40:09</t>
+  </si>
   <si>
     <t>Nombre</t>
   </si>
   <si>
-    <t>Concentracion</t>
-  </si>
-  <si>
-    <t>Adicional</t>
-  </si>
-  <si>
-    <t>Precio</t>
-  </si>
-  <si>
-    <t>Tipo</t>
-  </si>
-  <si>
-    <t>Presentacion</t>
-  </si>
-  <si>
-    <t>Laboratorio</t>
-  </si>
-  <si>
-    <t>buscapina ll</t>
+    <t>Concentración</t>
+  </si>
+  <si>
+    <t>buscapina ejemplo</t>
   </si>
   <si>
     <t>normal</t>
@@ -56,6 +47,21 @@
     <t>maria bd</t>
   </si>
   <si>
+    <t>Condones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">condones </t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>inyeccion</t>
+  </si>
+  <si>
+    <t>local host</t>
+  </si>
+  <si>
     <t>omeprosol</t>
   </si>
   <si>
@@ -78,9 +84,6 @@
   </si>
   <si>
     <t>wkjwfekj</t>
-  </si>
-  <si>
-    <t>inyeccion</t>
   </si>
   <si>
     <t>Bayer</t>
@@ -91,13 +94,22 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <b val="0"/>
       <i val="0"/>
       <strike val="0"/>
       <u val="none"/>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
@@ -119,9 +131,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -422,108 +440,141 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2">
-        <v>1.78</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3">
-        <v>1.5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>1.78</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6">
+        <v>1.5</v>
+      </c>
+      <c r="E6" t="s">
         <v>18</v>
       </c>
-      <c r="B4" t="s">
+      <c r="F6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
         <v>20</v>
       </c>
-      <c r="D4">
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7">
         <v>90</v>
       </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" t="s">
-        <v>22</v>
-      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <mergeCells>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="B3:C3"/>
+  </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
FEATURE:Report the project the farmacy
</commit_message>
<xml_diff>
--- a/excel/reporte_producto.xlsx
+++ b/excel/reporte_producto.xlsx
@@ -15,12 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
   <si>
     <t>Reporte de Ventas</t>
   </si>
   <si>
-    <t>Fecha  2021-11-18 15:40:09</t>
+    <t>Fecha  2023-02-04 22:13:24</t>
   </si>
   <si>
     <t>Nombre</t>
@@ -29,7 +29,22 @@
     <t>Concentración</t>
   </si>
   <si>
-    <t>buscapina ejemplo</t>
+    <t>Adicional</t>
+  </si>
+  <si>
+    <t>Precio</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Presentacion</t>
+  </si>
+  <si>
+    <t>Laboratorio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">buscapina </t>
   </si>
   <si>
     <t>normal</t>
@@ -56,7 +71,7 @@
     <t>c</t>
   </si>
   <si>
-    <t>inyeccion</t>
+    <t>Suero</t>
   </si>
   <si>
     <t>local host</t>
@@ -436,7 +451,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
@@ -465,97 +480,112 @@
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D4">
         <v>1.78</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G4" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
         <v>12</v>
       </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
-      </c>
       <c r="F5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G5" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D6">
         <v>1.5</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G6" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D7">
         <v>90</v>
       </c>
       <c r="E7" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -572,8 +602,6 @@
   <mergeCells>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="B3:C3"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
FIX:Integration the project with news features
</commit_message>
<xml_diff>
--- a/excel/reporte_producto.xlsx
+++ b/excel/reporte_producto.xlsx
@@ -15,12 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
   <si>
     <t>Reporte de Ventas</t>
   </si>
   <si>
-    <t>Fecha  2021-11-18 15:40:09</t>
+    <t>Fecha  2023-02-04 22:13:24</t>
   </si>
   <si>
     <t>Nombre</t>
@@ -29,7 +29,22 @@
     <t>Concentración</t>
   </si>
   <si>
-    <t>buscapina ejemplo</t>
+    <t>Adicional</t>
+  </si>
+  <si>
+    <t>Precio</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Presentacion</t>
+  </si>
+  <si>
+    <t>Laboratorio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">buscapina </t>
   </si>
   <si>
     <t>normal</t>
@@ -56,7 +71,7 @@
     <t>c</t>
   </si>
   <si>
-    <t>inyeccion</t>
+    <t>Suero</t>
   </si>
   <si>
     <t>local host</t>
@@ -436,7 +451,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
@@ -465,97 +480,112 @@
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D4">
         <v>1.78</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G4" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
         <v>12</v>
       </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
-      </c>
       <c r="F5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G5" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D6">
         <v>1.5</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G6" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D7">
         <v>90</v>
       </c>
       <c r="E7" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -572,8 +602,6 @@
   <mergeCells>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="B3:C3"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>